<commit_message>
Working so far, tweaked torso to be tighter with 4 cylinders
</commit_message>
<xml_diff>
--- a/Primitives.xlsx
+++ b/Primitives.xlsx
@@ -199,7 +199,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -218,6 +218,7 @@
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="2" fontId="5" numFmtId="165" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
@@ -236,12 +237,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.54117647058824"/>
+  </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
       <c r="A1" s="1"/>
@@ -604,6 +608,15 @@
         <f aca="false">11.5*(25.4/1000)</f>
         <v>0.2921</v>
       </c>
+      <c r="N12" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>1.25</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="13">
       <c r="A13" s="1" t="s">
@@ -636,6 +649,18 @@
         <f aca="false">11.5*(25.4/1000)</f>
         <v>0.2921</v>
       </c>
+      <c r="N13" s="15" t="n">
+        <f aca="false">N12*25.4/1000/2</f>
+        <v>0.1143</v>
+      </c>
+      <c r="O13" s="15" t="n">
+        <f aca="false">O12*25.4/1000</f>
+        <v>0.0508</v>
+      </c>
+      <c r="P13" s="15" t="n">
+        <f aca="false">P12*25.4/1000</f>
+        <v>0.03175</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="14">
       <c r="A14" s="1" t="s">
@@ -891,6 +916,12 @@
       <c r="I21" s="8" t="n">
         <f aca="false">3.75*(25.4/1000)</f>
         <v>0.09525</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="23">
+      <c r="M23" s="15" t="n">
+        <f aca="false">0.254/2/2</f>
+        <v>0.0635</v>
       </c>
     </row>
   </sheetData>
@@ -918,6 +949,9 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.54117647058824"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -940,6 +974,9 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.54117647058824"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>